<commit_message>
Add dbSUPER enhancer database
</commit_message>
<xml_diff>
--- a/GenomeRunner.xlsx
+++ b/GenomeRunner.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="32480" yWindow="5040" windowWidth="28800" windowHeight="16380" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="46180" yWindow="4880" windowWidth="28800" windowHeight="16380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data and Analysis" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="GWAS" sheetId="7" r:id="rId7"/>
     <sheet name="Histones" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5817" uniqueCount="1567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5822" uniqueCount="1570">
   <si>
     <t>Mitranscriptome</t>
   </si>
@@ -7174,12 +7174,6 @@
     <t>http://archive.gersteinlab.org/funseq2.1.0_data/</t>
   </si>
   <si>
-    <t>Misc data from Gerstein lab</t>
-  </si>
-  <si>
-    <t>misc</t>
-  </si>
-  <si>
     <t>DENdb</t>
   </si>
   <si>
@@ -7190,12 +7184,27 @@
   </si>
   <si>
     <t>hg19, ChIP-seq, DNAse, Enhancers, TFs, FANTOM expression</t>
+  </si>
+  <si>
+    <t>Misc annotation data for FunSeq2</t>
+  </si>
+  <si>
+    <t>misc, hg19</t>
+  </si>
+  <si>
+    <t>http://asntech.org/dbsuper/download.php</t>
+  </si>
+  <si>
+    <t>Super-enhancers, cell-/tissue-specific</t>
+  </si>
+  <si>
+    <t>BED files, hg19, mm9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -7462,6 +7471,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -8204,11 +8216,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G135"/>
+  <dimension ref="A1:G143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8737,507 +8749,389 @@
         <v>1560</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>1561</v>
+        <v>1565</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>1562</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
+        <v>1561</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>1563</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>1564</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>1565</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="4"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
+      <c r="A34" s="4" t="s">
+        <v>1552</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>1567</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>1568</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="4"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>112</v>
-      </c>
+      <c r="A36" s="4"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>119</v>
-      </c>
+      <c r="A37" s="4"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" s="4"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>120</v>
-      </c>
-      <c r="B39" t="s">
-        <v>121</v>
-      </c>
-      <c r="C39" t="s">
-        <v>122</v>
-      </c>
-      <c r="D39" t="s">
-        <v>123</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="G39" t="s">
-        <v>126</v>
-      </c>
+      <c r="A39" s="4"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>127</v>
-      </c>
-      <c r="B40" t="s">
-        <v>121</v>
-      </c>
-      <c r="C40" t="s">
-        <v>128</v>
-      </c>
-      <c r="D40" t="s">
-        <v>129</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="G40" t="s">
-        <v>130</v>
-      </c>
+      <c r="A40" s="4"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="B41" t="s">
-        <v>121</v>
-      </c>
-      <c r="C41" t="s">
-        <v>122</v>
-      </c>
-      <c r="D41" t="s">
-        <v>132</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="G41" t="s">
-        <v>134</v>
-      </c>
+      <c r="A41" s="4"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B42" t="s">
-        <v>121</v>
-      </c>
-      <c r="C42" t="s">
-        <v>122</v>
-      </c>
-      <c r="D42" t="s">
-        <v>132</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="G42" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>136</v>
-      </c>
-      <c r="B43" t="s">
-        <v>121</v>
-      </c>
-      <c r="C43" t="s">
-        <v>122</v>
-      </c>
-      <c r="D43" t="s">
-        <v>137</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="F43" t="s">
-        <v>138</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>139</v>
-      </c>
+      <c r="A42" s="4"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>140</v>
-      </c>
-      <c r="B44" t="s">
-        <v>140</v>
-      </c>
-      <c r="C44" t="s">
-        <v>122</v>
-      </c>
-      <c r="D44" t="s">
-        <v>141</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="F44" t="s">
-        <v>142</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>140</v>
-      </c>
-      <c r="B45" t="s">
-        <v>140</v>
-      </c>
-      <c r="C45" t="s">
-        <v>122</v>
-      </c>
-      <c r="D45" t="s">
-        <v>144</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="F45" t="s">
-        <v>142</v>
-      </c>
-      <c r="G45" s="9" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>140</v>
-      </c>
-      <c r="B46" t="s">
-        <v>140</v>
-      </c>
-      <c r="C46" t="s">
-        <v>122</v>
-      </c>
-      <c r="D46" t="s">
-        <v>145</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="F46" t="s">
-        <v>142</v>
-      </c>
-      <c r="G46" s="9" t="s">
-        <v>143</v>
+        <v>526</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="B47" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="C47" t="s">
         <v>122</v>
       </c>
       <c r="D47" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="F47" t="s">
-        <v>142</v>
-      </c>
-      <c r="G47" s="9" t="s">
-        <v>143</v>
+      <c r="F47" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G47" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="B48" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="C48" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D48" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="F48" t="s">
-        <v>142</v>
-      </c>
-      <c r="G48" s="9" t="s">
-        <v>143</v>
+      <c r="F48" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G48" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>148</v>
+      <c r="A49" s="8" t="s">
+        <v>131</v>
       </c>
       <c r="B49" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="C49" t="s">
         <v>122</v>
       </c>
       <c r="D49" t="s">
-        <v>149</v>
-      </c>
-      <c r="E49" t="s">
+        <v>132</v>
+      </c>
+      <c r="E49" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="F49" t="s">
-        <v>150</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>151</v>
+      <c r="F49" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="G49" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>152</v>
+      <c r="A50" s="8" t="s">
+        <v>135</v>
       </c>
       <c r="B50" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="C50" t="s">
         <v>122</v>
       </c>
       <c r="D50" t="s">
-        <v>153</v>
-      </c>
-      <c r="E50" t="s">
-        <v>154</v>
-      </c>
-      <c r="F50" t="s">
-        <v>155</v>
-      </c>
-      <c r="G50" s="9" t="s">
-        <v>156</v>
+        <v>132</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="G50" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="B51" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
       <c r="C51" t="s">
         <v>122</v>
       </c>
       <c r="D51" t="s">
-        <v>157</v>
-      </c>
-      <c r="E51" t="s">
-        <v>154</v>
+        <v>137</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="F51" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="B52" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C52" t="s">
         <v>122</v>
       </c>
       <c r="D52" t="s">
-        <v>159</v>
-      </c>
-      <c r="E52" t="s">
-        <v>160</v>
+        <v>141</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="F52" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="B53" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C53" t="s">
         <v>122</v>
       </c>
       <c r="D53" t="s">
-        <v>162</v>
-      </c>
-      <c r="E53" t="s">
-        <v>163</v>
+        <v>144</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="F53" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="B54" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C54" t="s">
         <v>122</v>
       </c>
       <c r="D54" t="s">
-        <v>165</v>
-      </c>
-      <c r="E54" t="s">
-        <v>166</v>
+        <v>145</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="F54" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="B55" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C55" t="s">
         <v>122</v>
       </c>
       <c r="D55" t="s">
-        <v>168</v>
-      </c>
-      <c r="E55" t="s">
-        <v>169</v>
+        <v>146</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="F55" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="B56" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C56" t="s">
         <v>122</v>
       </c>
       <c r="D56" t="s">
-        <v>171</v>
-      </c>
-      <c r="E56" t="s">
-        <v>172</v>
+        <v>147</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="F56" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B57" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C57" t="s">
         <v>122</v>
       </c>
       <c r="D57" t="s">
-        <v>174</v>
+        <v>149</v>
       </c>
       <c r="E57" t="s">
-        <v>175</v>
+        <v>124</v>
       </c>
       <c r="F57" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -9251,16 +9145,16 @@
         <v>122</v>
       </c>
       <c r="D58" t="s">
-        <v>177</v>
+        <v>153</v>
       </c>
       <c r="E58" t="s">
-        <v>178</v>
+        <v>154</v>
       </c>
       <c r="F58" t="s">
         <v>155</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -9274,16 +9168,16 @@
         <v>122</v>
       </c>
       <c r="D59" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="E59" t="s">
-        <v>181</v>
+        <v>154</v>
       </c>
       <c r="F59" t="s">
         <v>155</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -9297,16 +9191,16 @@
         <v>122</v>
       </c>
       <c r="D60" t="s">
-        <v>183</v>
+        <v>159</v>
       </c>
       <c r="E60" t="s">
-        <v>184</v>
+        <v>160</v>
       </c>
       <c r="F60" t="s">
         <v>155</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>185</v>
+        <v>161</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -9320,16 +9214,16 @@
         <v>122</v>
       </c>
       <c r="D61" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="E61" t="s">
-        <v>187</v>
+        <v>163</v>
       </c>
       <c r="F61" t="s">
         <v>155</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>188</v>
+        <v>164</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -9343,16 +9237,16 @@
         <v>122</v>
       </c>
       <c r="D62" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="E62" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="F62" t="s">
         <v>155</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -9366,16 +9260,16 @@
         <v>122</v>
       </c>
       <c r="D63" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="E63" t="s">
-        <v>193</v>
+        <v>169</v>
       </c>
       <c r="F63" t="s">
         <v>155</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -9389,16 +9283,16 @@
         <v>122</v>
       </c>
       <c r="D64" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="E64" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="F64" t="s">
         <v>155</v>
       </c>
       <c r="G64" s="9" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -9412,16 +9306,16 @@
         <v>122</v>
       </c>
       <c r="D65" t="s">
-        <v>198</v>
+        <v>174</v>
       </c>
       <c r="E65" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="F65" t="s">
         <v>155</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -9435,16 +9329,16 @@
         <v>122</v>
       </c>
       <c r="D66" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="E66" t="s">
-        <v>202</v>
+        <v>178</v>
       </c>
       <c r="F66" t="s">
         <v>155</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>203</v>
+        <v>179</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -9458,16 +9352,16 @@
         <v>122</v>
       </c>
       <c r="D67" t="s">
-        <v>204</v>
+        <v>180</v>
       </c>
       <c r="E67" t="s">
-        <v>205</v>
+        <v>181</v>
       </c>
       <c r="F67" t="s">
         <v>155</v>
       </c>
       <c r="G67" s="9" t="s">
-        <v>206</v>
+        <v>182</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -9481,16 +9375,16 @@
         <v>122</v>
       </c>
       <c r="D68" t="s">
-        <v>207</v>
+        <v>183</v>
       </c>
       <c r="E68" t="s">
-        <v>208</v>
+        <v>184</v>
       </c>
       <c r="F68" t="s">
         <v>155</v>
       </c>
       <c r="G68" s="9" t="s">
-        <v>209</v>
+        <v>185</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -9504,16 +9398,16 @@
         <v>122</v>
       </c>
       <c r="D69" t="s">
-        <v>210</v>
+        <v>186</v>
       </c>
       <c r="E69" t="s">
-        <v>211</v>
+        <v>187</v>
       </c>
       <c r="F69" t="s">
         <v>155</v>
       </c>
       <c r="G69" s="9" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -9527,16 +9421,16 @@
         <v>122</v>
       </c>
       <c r="D70" t="s">
-        <v>213</v>
+        <v>189</v>
       </c>
       <c r="E70" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="F70" t="s">
         <v>155</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
@@ -9550,16 +9444,16 @@
         <v>122</v>
       </c>
       <c r="D71" t="s">
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="E71" t="s">
-        <v>217</v>
+        <v>193</v>
       </c>
       <c r="F71" t="s">
         <v>155</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>218</v>
+        <v>194</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -9573,16 +9467,16 @@
         <v>122</v>
       </c>
       <c r="D72" t="s">
-        <v>219</v>
+        <v>195</v>
       </c>
       <c r="E72" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="F72" t="s">
         <v>155</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>221</v>
+        <v>197</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -9596,16 +9490,16 @@
         <v>122</v>
       </c>
       <c r="D73" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="E73" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="F73" t="s">
         <v>155</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -9619,16 +9513,16 @@
         <v>122</v>
       </c>
       <c r="D74" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="E74" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="F74" t="s">
         <v>155</v>
       </c>
       <c r="G74" s="9" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -9642,16 +9536,16 @@
         <v>122</v>
       </c>
       <c r="D75" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="E75" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="F75" t="s">
         <v>155</v>
       </c>
       <c r="G75" s="9" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -9665,16 +9559,16 @@
         <v>122</v>
       </c>
       <c r="D76" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="E76" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="F76" t="s">
         <v>155</v>
       </c>
       <c r="G76" s="9" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
@@ -9688,16 +9582,16 @@
         <v>122</v>
       </c>
       <c r="D77" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="E77" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="F77" t="s">
         <v>155</v>
       </c>
       <c r="G77" s="9" t="s">
-        <v>236</v>
+        <v>212</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -9711,16 +9605,16 @@
         <v>122</v>
       </c>
       <c r="D78" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="E78" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="F78" t="s">
         <v>155</v>
       </c>
       <c r="G78" s="9" t="s">
-        <v>239</v>
+        <v>215</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
@@ -9734,16 +9628,16 @@
         <v>122</v>
       </c>
       <c r="D79" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
       <c r="E79" t="s">
-        <v>241</v>
+        <v>217</v>
       </c>
       <c r="F79" t="s">
         <v>155</v>
       </c>
       <c r="G79" s="9" t="s">
-        <v>242</v>
+        <v>218</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -9757,16 +9651,16 @@
         <v>122</v>
       </c>
       <c r="D80" t="s">
-        <v>243</v>
+        <v>219</v>
       </c>
       <c r="E80" t="s">
-        <v>244</v>
+        <v>220</v>
       </c>
       <c r="F80" t="s">
         <v>155</v>
       </c>
       <c r="G80" s="9" t="s">
-        <v>245</v>
+        <v>221</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -9780,16 +9674,16 @@
         <v>122</v>
       </c>
       <c r="D81" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="E81" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="F81" t="s">
         <v>155</v>
       </c>
       <c r="G81" s="9" t="s">
-        <v>248</v>
+        <v>224</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -9803,16 +9697,16 @@
         <v>122</v>
       </c>
       <c r="D82" t="s">
-        <v>249</v>
+        <v>225</v>
       </c>
       <c r="E82" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="F82" t="s">
         <v>155</v>
       </c>
       <c r="G82" s="9" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -9826,16 +9720,16 @@
         <v>122</v>
       </c>
       <c r="D83" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="E83" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="F83" t="s">
         <v>155</v>
       </c>
       <c r="G83" s="9" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
@@ -9849,16 +9743,16 @@
         <v>122</v>
       </c>
       <c r="D84" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="E84" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="F84" t="s">
         <v>155</v>
       </c>
       <c r="G84" s="9" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -9872,16 +9766,16 @@
         <v>122</v>
       </c>
       <c r="D85" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
       <c r="E85" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="F85" t="s">
         <v>155</v>
       </c>
       <c r="G85" s="9" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
@@ -9895,16 +9789,16 @@
         <v>122</v>
       </c>
       <c r="D86" t="s">
-        <v>261</v>
+        <v>237</v>
       </c>
       <c r="E86" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="F86" t="s">
         <v>155</v>
       </c>
       <c r="G86" s="9" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
@@ -9918,16 +9812,16 @@
         <v>122</v>
       </c>
       <c r="D87" t="s">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="E87" t="s">
-        <v>265</v>
+        <v>241</v>
       </c>
       <c r="F87" t="s">
         <v>155</v>
       </c>
       <c r="G87" s="9" t="s">
-        <v>266</v>
+        <v>242</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -9941,16 +9835,16 @@
         <v>122</v>
       </c>
       <c r="D88" t="s">
-        <v>267</v>
+        <v>243</v>
       </c>
       <c r="E88" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
       <c r="F88" t="s">
         <v>155</v>
       </c>
       <c r="G88" s="9" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -9964,16 +9858,16 @@
         <v>122</v>
       </c>
       <c r="D89" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="E89" t="s">
-        <v>271</v>
+        <v>247</v>
       </c>
       <c r="F89" t="s">
         <v>155</v>
       </c>
       <c r="G89" s="9" t="s">
-        <v>272</v>
+        <v>248</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
@@ -9987,16 +9881,16 @@
         <v>122</v>
       </c>
       <c r="D90" t="s">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="E90" t="s">
-        <v>274</v>
+        <v>250</v>
       </c>
       <c r="F90" t="s">
         <v>155</v>
       </c>
       <c r="G90" s="9" t="s">
-        <v>275</v>
+        <v>251</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -10010,16 +9904,16 @@
         <v>122</v>
       </c>
       <c r="D91" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="E91" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
       <c r="F91" t="s">
         <v>155</v>
       </c>
       <c r="G91" s="9" t="s">
-        <v>278</v>
+        <v>254</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
@@ -10033,16 +9927,16 @@
         <v>122</v>
       </c>
       <c r="D92" t="s">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="E92" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
       <c r="F92" t="s">
         <v>155</v>
       </c>
       <c r="G92" s="9" t="s">
-        <v>281</v>
+        <v>257</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
@@ -10056,16 +9950,16 @@
         <v>122</v>
       </c>
       <c r="D93" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
       <c r="E93" t="s">
-        <v>283</v>
+        <v>259</v>
       </c>
       <c r="F93" t="s">
         <v>155</v>
       </c>
       <c r="G93" s="9" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -10079,16 +9973,16 @@
         <v>122</v>
       </c>
       <c r="D94" t="s">
-        <v>285</v>
+        <v>261</v>
       </c>
       <c r="E94" t="s">
-        <v>286</v>
+        <v>262</v>
       </c>
       <c r="F94" t="s">
         <v>155</v>
       </c>
       <c r="G94" s="9" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -10102,16 +9996,16 @@
         <v>122</v>
       </c>
       <c r="D95" t="s">
-        <v>288</v>
+        <v>264</v>
       </c>
       <c r="E95" t="s">
-        <v>289</v>
+        <v>265</v>
       </c>
       <c r="F95" t="s">
         <v>155</v>
       </c>
       <c r="G95" s="9" t="s">
-        <v>290</v>
+        <v>266</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
@@ -10125,16 +10019,16 @@
         <v>122</v>
       </c>
       <c r="D96" t="s">
-        <v>291</v>
+        <v>267</v>
       </c>
       <c r="E96" t="s">
-        <v>292</v>
+        <v>268</v>
       </c>
       <c r="F96" t="s">
         <v>155</v>
       </c>
       <c r="G96" s="9" t="s">
-        <v>293</v>
+        <v>269</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -10148,16 +10042,16 @@
         <v>122</v>
       </c>
       <c r="D97" t="s">
-        <v>294</v>
+        <v>270</v>
       </c>
       <c r="E97" t="s">
-        <v>295</v>
+        <v>271</v>
       </c>
       <c r="F97" t="s">
         <v>155</v>
       </c>
       <c r="G97" s="9" t="s">
-        <v>296</v>
+        <v>272</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
@@ -10171,16 +10065,16 @@
         <v>122</v>
       </c>
       <c r="D98" t="s">
-        <v>297</v>
+        <v>273</v>
       </c>
       <c r="E98" t="s">
-        <v>298</v>
+        <v>274</v>
       </c>
       <c r="F98" t="s">
         <v>155</v>
       </c>
       <c r="G98" s="9" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
@@ -10194,16 +10088,16 @@
         <v>122</v>
       </c>
       <c r="D99" t="s">
-        <v>300</v>
+        <v>276</v>
       </c>
       <c r="E99" t="s">
-        <v>301</v>
+        <v>277</v>
       </c>
       <c r="F99" t="s">
         <v>155</v>
       </c>
       <c r="G99" s="9" t="s">
-        <v>302</v>
+        <v>278</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
@@ -10217,16 +10111,16 @@
         <v>122</v>
       </c>
       <c r="D100" t="s">
-        <v>303</v>
+        <v>279</v>
       </c>
       <c r="E100" t="s">
-        <v>304</v>
+        <v>280</v>
       </c>
       <c r="F100" t="s">
         <v>155</v>
       </c>
       <c r="G100" s="9" t="s">
-        <v>305</v>
+        <v>281</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -10240,16 +10134,16 @@
         <v>122</v>
       </c>
       <c r="D101" t="s">
-        <v>306</v>
+        <v>282</v>
       </c>
       <c r="E101" t="s">
-        <v>307</v>
+        <v>283</v>
       </c>
       <c r="F101" t="s">
         <v>155</v>
       </c>
       <c r="G101" s="9" t="s">
-        <v>308</v>
+        <v>284</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
@@ -10263,16 +10157,16 @@
         <v>122</v>
       </c>
       <c r="D102" t="s">
-        <v>309</v>
+        <v>285</v>
       </c>
       <c r="E102" t="s">
-        <v>310</v>
+        <v>286</v>
       </c>
       <c r="F102" t="s">
         <v>155</v>
       </c>
       <c r="G102" s="9" t="s">
-        <v>311</v>
+        <v>287</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
@@ -10286,16 +10180,16 @@
         <v>122</v>
       </c>
       <c r="D103" t="s">
-        <v>312</v>
+        <v>288</v>
       </c>
       <c r="E103" t="s">
-        <v>313</v>
+        <v>289</v>
       </c>
       <c r="F103" t="s">
         <v>155</v>
       </c>
       <c r="G103" s="9" t="s">
-        <v>314</v>
+        <v>290</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
@@ -10309,16 +10203,16 @@
         <v>122</v>
       </c>
       <c r="D104" t="s">
-        <v>315</v>
+        <v>291</v>
       </c>
       <c r="E104" t="s">
-        <v>316</v>
+        <v>292</v>
       </c>
       <c r="F104" t="s">
         <v>155</v>
       </c>
       <c r="G104" s="9" t="s">
-        <v>317</v>
+        <v>293</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.2">
@@ -10332,16 +10226,16 @@
         <v>122</v>
       </c>
       <c r="D105" t="s">
-        <v>318</v>
+        <v>294</v>
       </c>
       <c r="E105" t="s">
-        <v>319</v>
+        <v>295</v>
       </c>
       <c r="F105" t="s">
         <v>155</v>
       </c>
       <c r="G105" s="9" t="s">
-        <v>320</v>
+        <v>296</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
@@ -10355,16 +10249,16 @@
         <v>122</v>
       </c>
       <c r="D106" t="s">
-        <v>321</v>
+        <v>297</v>
       </c>
       <c r="E106" t="s">
-        <v>322</v>
+        <v>298</v>
       </c>
       <c r="F106" t="s">
         <v>155</v>
       </c>
       <c r="G106" s="9" t="s">
-        <v>323</v>
+        <v>299</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
@@ -10378,16 +10272,16 @@
         <v>122</v>
       </c>
       <c r="D107" t="s">
-        <v>324</v>
+        <v>300</v>
       </c>
       <c r="E107" t="s">
-        <v>325</v>
+        <v>301</v>
       </c>
       <c r="F107" t="s">
         <v>155</v>
       </c>
       <c r="G107" s="9" t="s">
-        <v>326</v>
+        <v>302</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
@@ -10401,16 +10295,16 @@
         <v>122</v>
       </c>
       <c r="D108" t="s">
-        <v>327</v>
+        <v>303</v>
       </c>
       <c r="E108" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="F108" t="s">
         <v>155</v>
       </c>
       <c r="G108" s="9" t="s">
-        <v>329</v>
+        <v>305</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.2">
@@ -10424,16 +10318,16 @@
         <v>122</v>
       </c>
       <c r="D109" t="s">
-        <v>330</v>
+        <v>306</v>
       </c>
       <c r="E109" t="s">
-        <v>331</v>
+        <v>307</v>
       </c>
       <c r="F109" t="s">
         <v>155</v>
       </c>
       <c r="G109" s="9" t="s">
-        <v>332</v>
+        <v>308</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
@@ -10447,16 +10341,16 @@
         <v>122</v>
       </c>
       <c r="D110" t="s">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="E110" t="s">
-        <v>334</v>
+        <v>310</v>
       </c>
       <c r="F110" t="s">
         <v>155</v>
       </c>
       <c r="G110" s="9" t="s">
-        <v>335</v>
+        <v>311</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
@@ -10470,16 +10364,16 @@
         <v>122</v>
       </c>
       <c r="D111" t="s">
-        <v>336</v>
+        <v>312</v>
       </c>
       <c r="E111" t="s">
-        <v>337</v>
+        <v>313</v>
       </c>
       <c r="F111" t="s">
         <v>155</v>
       </c>
       <c r="G111" s="9" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
@@ -10493,16 +10387,16 @@
         <v>122</v>
       </c>
       <c r="D112" t="s">
-        <v>339</v>
+        <v>315</v>
       </c>
       <c r="E112" t="s">
-        <v>340</v>
+        <v>316</v>
       </c>
       <c r="F112" t="s">
         <v>155</v>
       </c>
       <c r="G112" s="9" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
@@ -10516,16 +10410,16 @@
         <v>122</v>
       </c>
       <c r="D113" t="s">
-        <v>342</v>
+        <v>318</v>
       </c>
       <c r="E113" t="s">
-        <v>343</v>
+        <v>319</v>
       </c>
       <c r="F113" t="s">
         <v>155</v>
       </c>
       <c r="G113" s="9" t="s">
-        <v>344</v>
+        <v>320</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
@@ -10539,16 +10433,16 @@
         <v>122</v>
       </c>
       <c r="D114" t="s">
-        <v>345</v>
+        <v>321</v>
       </c>
       <c r="E114" t="s">
-        <v>346</v>
+        <v>322</v>
       </c>
       <c r="F114" t="s">
         <v>155</v>
       </c>
       <c r="G114" s="9" t="s">
-        <v>347</v>
+        <v>323</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
@@ -10562,16 +10456,16 @@
         <v>122</v>
       </c>
       <c r="D115" t="s">
-        <v>348</v>
+        <v>324</v>
       </c>
       <c r="E115" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="F115" t="s">
         <v>155</v>
       </c>
       <c r="G115" s="9" t="s">
-        <v>350</v>
+        <v>326</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
@@ -10585,16 +10479,16 @@
         <v>122</v>
       </c>
       <c r="D116" t="s">
-        <v>351</v>
+        <v>327</v>
       </c>
       <c r="E116" t="s">
-        <v>352</v>
+        <v>328</v>
       </c>
       <c r="F116" t="s">
         <v>155</v>
       </c>
       <c r="G116" s="9" t="s">
-        <v>353</v>
+        <v>329</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
@@ -10608,16 +10502,16 @@
         <v>122</v>
       </c>
       <c r="D117" t="s">
-        <v>354</v>
+        <v>330</v>
       </c>
       <c r="E117" t="s">
-        <v>355</v>
+        <v>331</v>
       </c>
       <c r="F117" t="s">
         <v>155</v>
       </c>
       <c r="G117" s="9" t="s">
-        <v>356</v>
+        <v>332</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
@@ -10631,16 +10525,16 @@
         <v>122</v>
       </c>
       <c r="D118" t="s">
-        <v>357</v>
+        <v>333</v>
       </c>
       <c r="E118" t="s">
-        <v>358</v>
+        <v>334</v>
       </c>
       <c r="F118" t="s">
         <v>155</v>
       </c>
       <c r="G118" s="9" t="s">
-        <v>359</v>
+        <v>335</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
@@ -10654,16 +10548,16 @@
         <v>122</v>
       </c>
       <c r="D119" t="s">
-        <v>360</v>
+        <v>336</v>
       </c>
       <c r="E119" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="F119" t="s">
         <v>155</v>
       </c>
       <c r="G119" s="9" t="s">
-        <v>362</v>
+        <v>338</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
@@ -10677,16 +10571,16 @@
         <v>122</v>
       </c>
       <c r="D120" t="s">
-        <v>363</v>
+        <v>339</v>
       </c>
       <c r="E120" t="s">
-        <v>364</v>
+        <v>340</v>
       </c>
       <c r="F120" t="s">
         <v>155</v>
       </c>
       <c r="G120" s="9" t="s">
-        <v>365</v>
+        <v>341</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
@@ -10700,16 +10594,16 @@
         <v>122</v>
       </c>
       <c r="D121" t="s">
-        <v>366</v>
+        <v>342</v>
       </c>
       <c r="E121" t="s">
-        <v>367</v>
+        <v>343</v>
       </c>
       <c r="F121" t="s">
         <v>155</v>
       </c>
       <c r="G121" s="9" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
@@ -10723,16 +10617,16 @@
         <v>122</v>
       </c>
       <c r="D122" t="s">
-        <v>369</v>
+        <v>345</v>
       </c>
       <c r="E122" t="s">
-        <v>370</v>
+        <v>346</v>
       </c>
       <c r="F122" t="s">
         <v>155</v>
       </c>
       <c r="G122" s="9" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
@@ -10746,16 +10640,16 @@
         <v>122</v>
       </c>
       <c r="D123" t="s">
-        <v>372</v>
+        <v>348</v>
       </c>
       <c r="E123" t="s">
-        <v>373</v>
+        <v>349</v>
       </c>
       <c r="F123" t="s">
         <v>155</v>
       </c>
       <c r="G123" s="9" t="s">
-        <v>374</v>
+        <v>350</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
@@ -10769,16 +10663,16 @@
         <v>122</v>
       </c>
       <c r="D124" t="s">
-        <v>375</v>
+        <v>351</v>
       </c>
       <c r="E124" t="s">
-        <v>376</v>
+        <v>352</v>
       </c>
       <c r="F124" t="s">
         <v>155</v>
       </c>
       <c r="G124" s="9" t="s">
-        <v>377</v>
+        <v>353</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
@@ -10792,16 +10686,16 @@
         <v>122</v>
       </c>
       <c r="D125" t="s">
-        <v>378</v>
+        <v>354</v>
       </c>
       <c r="E125" t="s">
-        <v>379</v>
+        <v>355</v>
       </c>
       <c r="F125" t="s">
         <v>155</v>
       </c>
       <c r="G125" s="9" t="s">
-        <v>380</v>
+        <v>356</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
@@ -10815,16 +10709,16 @@
         <v>122</v>
       </c>
       <c r="D126" t="s">
-        <v>381</v>
+        <v>357</v>
       </c>
       <c r="E126" t="s">
-        <v>382</v>
+        <v>358</v>
       </c>
       <c r="F126" t="s">
         <v>155</v>
       </c>
       <c r="G126" s="9" t="s">
-        <v>383</v>
+        <v>359</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
@@ -10838,16 +10732,16 @@
         <v>122</v>
       </c>
       <c r="D127" t="s">
-        <v>384</v>
+        <v>360</v>
       </c>
       <c r="E127" t="s">
-        <v>385</v>
+        <v>361</v>
       </c>
       <c r="F127" t="s">
         <v>155</v>
       </c>
       <c r="G127" s="9" t="s">
-        <v>386</v>
+        <v>362</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
@@ -10861,16 +10755,16 @@
         <v>122</v>
       </c>
       <c r="D128" t="s">
-        <v>387</v>
+        <v>363</v>
       </c>
       <c r="E128" t="s">
-        <v>388</v>
+        <v>364</v>
       </c>
       <c r="F128" t="s">
         <v>155</v>
       </c>
       <c r="G128" s="9" t="s">
-        <v>389</v>
+        <v>365</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
@@ -10884,16 +10778,16 @@
         <v>122</v>
       </c>
       <c r="D129" t="s">
-        <v>390</v>
+        <v>366</v>
       </c>
       <c r="E129" t="s">
-        <v>391</v>
+        <v>367</v>
       </c>
       <c r="F129" t="s">
         <v>155</v>
       </c>
       <c r="G129" s="9" t="s">
-        <v>392</v>
+        <v>368</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
@@ -10907,16 +10801,16 @@
         <v>122</v>
       </c>
       <c r="D130" t="s">
-        <v>393</v>
+        <v>369</v>
       </c>
       <c r="E130" t="s">
-        <v>394</v>
+        <v>370</v>
       </c>
       <c r="F130" t="s">
         <v>155</v>
       </c>
       <c r="G130" s="9" t="s">
-        <v>395</v>
+        <v>371</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
@@ -10930,16 +10824,16 @@
         <v>122</v>
       </c>
       <c r="D131" t="s">
-        <v>396</v>
+        <v>372</v>
       </c>
       <c r="E131" t="s">
-        <v>397</v>
+        <v>373</v>
       </c>
       <c r="F131" t="s">
         <v>155</v>
       </c>
       <c r="G131" s="9" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
@@ -10953,16 +10847,16 @@
         <v>122</v>
       </c>
       <c r="D132" t="s">
-        <v>399</v>
+        <v>375</v>
       </c>
       <c r="E132" t="s">
-        <v>400</v>
+        <v>376</v>
       </c>
       <c r="F132" t="s">
         <v>155</v>
       </c>
       <c r="G132" s="9" t="s">
-        <v>401</v>
+        <v>377</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
@@ -10976,16 +10870,16 @@
         <v>122</v>
       </c>
       <c r="D133" t="s">
-        <v>402</v>
+        <v>378</v>
       </c>
       <c r="E133" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="F133" t="s">
         <v>155</v>
       </c>
       <c r="G133" s="9" t="s">
-        <v>404</v>
+        <v>380</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
@@ -10999,16 +10893,16 @@
         <v>122</v>
       </c>
       <c r="D134" t="s">
-        <v>405</v>
+        <v>381</v>
       </c>
       <c r="E134" t="s">
-        <v>406</v>
+        <v>382</v>
       </c>
       <c r="F134" t="s">
         <v>155</v>
       </c>
       <c r="G134" s="9" t="s">
-        <v>407</v>
+        <v>383</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
@@ -11022,15 +10916,199 @@
         <v>122</v>
       </c>
       <c r="D135" t="s">
-        <v>408</v>
+        <v>384</v>
       </c>
       <c r="E135" t="s">
-        <v>409</v>
+        <v>385</v>
       </c>
       <c r="F135" t="s">
         <v>155</v>
       </c>
       <c r="G135" s="9" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>152</v>
+      </c>
+      <c r="B136" t="s">
+        <v>152</v>
+      </c>
+      <c r="C136" t="s">
+        <v>122</v>
+      </c>
+      <c r="D136" t="s">
+        <v>387</v>
+      </c>
+      <c r="E136" t="s">
+        <v>388</v>
+      </c>
+      <c r="F136" t="s">
+        <v>155</v>
+      </c>
+      <c r="G136" s="9" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>152</v>
+      </c>
+      <c r="B137" t="s">
+        <v>152</v>
+      </c>
+      <c r="C137" t="s">
+        <v>122</v>
+      </c>
+      <c r="D137" t="s">
+        <v>390</v>
+      </c>
+      <c r="E137" t="s">
+        <v>391</v>
+      </c>
+      <c r="F137" t="s">
+        <v>155</v>
+      </c>
+      <c r="G137" s="9" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>152</v>
+      </c>
+      <c r="B138" t="s">
+        <v>152</v>
+      </c>
+      <c r="C138" t="s">
+        <v>122</v>
+      </c>
+      <c r="D138" t="s">
+        <v>393</v>
+      </c>
+      <c r="E138" t="s">
+        <v>394</v>
+      </c>
+      <c r="F138" t="s">
+        <v>155</v>
+      </c>
+      <c r="G138" s="9" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>152</v>
+      </c>
+      <c r="B139" t="s">
+        <v>152</v>
+      </c>
+      <c r="C139" t="s">
+        <v>122</v>
+      </c>
+      <c r="D139" t="s">
+        <v>396</v>
+      </c>
+      <c r="E139" t="s">
+        <v>397</v>
+      </c>
+      <c r="F139" t="s">
+        <v>155</v>
+      </c>
+      <c r="G139" s="9" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>152</v>
+      </c>
+      <c r="B140" t="s">
+        <v>152</v>
+      </c>
+      <c r="C140" t="s">
+        <v>122</v>
+      </c>
+      <c r="D140" t="s">
+        <v>399</v>
+      </c>
+      <c r="E140" t="s">
+        <v>400</v>
+      </c>
+      <c r="F140" t="s">
+        <v>155</v>
+      </c>
+      <c r="G140" s="9" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>152</v>
+      </c>
+      <c r="B141" t="s">
+        <v>152</v>
+      </c>
+      <c r="C141" t="s">
+        <v>122</v>
+      </c>
+      <c r="D141" t="s">
+        <v>402</v>
+      </c>
+      <c r="E141" t="s">
+        <v>403</v>
+      </c>
+      <c r="F141" t="s">
+        <v>155</v>
+      </c>
+      <c r="G141" s="9" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>152</v>
+      </c>
+      <c r="B142" t="s">
+        <v>152</v>
+      </c>
+      <c r="C142" t="s">
+        <v>122</v>
+      </c>
+      <c r="D142" t="s">
+        <v>405</v>
+      </c>
+      <c r="E142" t="s">
+        <v>406</v>
+      </c>
+      <c r="F142" t="s">
+        <v>155</v>
+      </c>
+      <c r="G142" s="9" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>152</v>
+      </c>
+      <c r="B143" t="s">
+        <v>152</v>
+      </c>
+      <c r="C143" t="s">
+        <v>122</v>
+      </c>
+      <c r="D143" t="s">
+        <v>408</v>
+      </c>
+      <c r="E143" t="s">
+        <v>409</v>
+      </c>
+      <c r="F143" t="s">
+        <v>155</v>
+      </c>
+      <c r="G143" s="9" t="s">
         <v>410</v>
       </c>
     </row>
@@ -11062,6 +11140,7 @@
     <hyperlink ref="B25" r:id="rId24"/>
     <hyperlink ref="B31" r:id="rId25"/>
     <hyperlink ref="B33" r:id="rId26"/>
+    <hyperlink ref="B34" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Add GTRD TFBS ChIP-seq database
</commit_message>
<xml_diff>
--- a/GenomeRunner.xlsx
+++ b/GenomeRunner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10814"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdozmorov/Documents/Work/GenomeRunner/R.GenomeRunner/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E7F5CBE6-2D77-8A41-8AD8-7556588BE8AD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E8C90C-DB02-2A45-ADCC-CEEA03FF72FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31940" yWindow="1300" windowWidth="28800" windowHeight="16260" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5832" uniqueCount="1577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5837" uniqueCount="1581">
   <si>
     <t>Mitranscriptome</t>
   </si>
@@ -7399,6 +7399,18 @@
   </si>
   <si>
     <t>BED files, hg18, hg38</t>
+  </si>
+  <si>
+    <t>GTRD</t>
+  </si>
+  <si>
+    <t>http://gtrd.biouml.org/</t>
+  </si>
+  <si>
+    <t>Uniformly processed TFBSs, meta-clusters and cell type-specific</t>
+  </si>
+  <si>
+    <t>BED files, hg38, mm38</t>
   </si>
 </sst>
 </file>
@@ -8426,7 +8438,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9033,11 +9045,21 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="4"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
+      <c r="A37" s="4" t="s">
+        <v>1577</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>1578</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>1579</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>1580</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>

</xml_diff>